<commit_message>
most achievements implemented, working newgrounds medal stuff
</commit_message>
<xml_diff>
--- a/Promo/achievements.xlsx
+++ b/Promo/achievements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>nil *</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -419,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:F31"/>
+  <dimension ref="A5:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +433,7 @@
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -438,7 +441,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -450,7 +456,10 @@
         <v>480</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -458,7 +467,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -466,7 +478,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -474,7 +489,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -482,7 +500,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -490,7 +511,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
@@ -498,7 +522,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
@@ -506,7 +533,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
@@ -514,7 +544,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -522,7 +555,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
@@ -530,7 +566,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -538,7 +577,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
@@ -546,7 +588,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
       <c r="B19" t="s">
         <v>20</v>
       </c>
@@ -554,7 +599,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
       <c r="B20" t="s">
         <v>21</v>
       </c>
@@ -562,7 +610,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
       <c r="B21" t="s">
         <v>22</v>
       </c>
@@ -570,7 +621,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -578,7 +632,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
       <c r="B23" t="s">
         <v>24</v>
       </c>
@@ -586,7 +643,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>25</v>
       </c>
@@ -594,7 +651,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>6</v>
       </c>
@@ -602,7 +659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>7</v>
       </c>
@@ -610,7 +667,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
       <c r="B28" t="s">
         <v>8</v>
       </c>
@@ -618,7 +678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>9</v>
       </c>
@@ -626,7 +686,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
all of the other achievements implemented. temp scenes for ending stuff
</commit_message>
<xml_diff>
--- a/Promo/achievements.xlsx
+++ b/Promo/achievements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -425,7 +425,7 @@
   <dimension ref="A5:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,6 +644,9 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
       <c r="B25" t="s">
         <v>25</v>
       </c>
@@ -652,6 +655,9 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
       <c r="B26" t="s">
         <v>6</v>
       </c>
@@ -660,6 +666,9 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
@@ -679,6 +688,9 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
       <c r="B30" t="s">
         <v>9</v>
       </c>
@@ -687,6 +699,9 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
       <c r="B31" t="s">
         <v>10</v>
       </c>

</xml_diff>